<commit_message>
feat: math hw 5 edited
</commit_message>
<xml_diff>
--- a/Математика/ДЗ_5.xlsx
+++ b/Математика/ДЗ_5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\omstu-works-2\Математика\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tony_\OneDrive\Документы\omstu-works-2\Математика\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1829EF-C2AB-4D48-99C8-D2E0E22A2E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396F5D0C-D2B6-41AB-AB86-CCF36A522F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Многочлен Лагранжа" sheetId="1" r:id="rId1"/>
@@ -30,12 +30,15 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>Вариант 26</t>
   </si>
@@ -119,6 +122,39 @@
   </si>
   <si>
     <t>Первая формула Ньютона</t>
+  </si>
+  <si>
+    <t>y0*((x-x1)(x-x2)(x-x3)(x-x4)/(x0-x1)(x0-x2)(x0-x3)(x0-x4))</t>
+  </si>
+  <si>
+    <t>y1*((x-x0)(x-x2)(x-x3)(x-x4)/(x1-x0)(x1-x2)(x1-x3)(x1-x4))</t>
+  </si>
+  <si>
+    <t>y2*((x-x0)(x-x1)(x-x3)(x-x4)/(x2-x0)(x2-x1)(x2-x3)(x2-x4))</t>
+  </si>
+  <si>
+    <t>y3*((x-x0)(x-x1)(x-x2)(x-x4)/(x3-x0)(x3-x1)(x3-x2)(x3-x4))</t>
+  </si>
+  <si>
+    <t>y4*((x-x0)(x-x1)(x-x2)(x-x3)/(x4-x0)(x4-x1)(x4-x2)(x4-x3))</t>
+  </si>
+  <si>
+    <t>x^4</t>
+  </si>
+  <si>
+    <t>x^3</t>
+  </si>
+  <si>
+    <t>x^2</t>
+  </si>
+  <si>
+    <t>x^1</t>
+  </si>
+  <si>
+    <t>x^0</t>
+  </si>
+  <si>
+    <t>L сокращенный</t>
   </si>
 </sst>
 </file>
@@ -291,7 +327,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -498,6 +534,70 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-4625-448C-89F9-A88E48B0F340}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>L сокращённый</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Многочлен Лагранжа'!$I$18:$I$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-0.91169999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.94344609374999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.96189999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.97100234374999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.97370000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.97194609374999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.96669999999999989</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.95792734374999988</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.9446</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.91169999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AD8A-45DD-87BB-8490BBC618A8}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -554,7 +654,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2033121040"/>
@@ -613,7 +713,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2033120208"/>
@@ -654,7 +754,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1525,38 +1625,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:B9"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -1565,7 +1666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1577,7 +1678,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -1590,7 +1691,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <f>A8+0.2</f>
         <v>0.2</v>
@@ -1604,7 +1705,7 @@
         <v>0.30000000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <f t="shared" ref="A10:A12" si="2">A9+0.2</f>
         <v>0.4</v>
@@ -1618,7 +1719,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <f t="shared" si="2"/>
         <v>0.60000000000000009</v>
@@ -1632,7 +1733,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <f t="shared" si="2"/>
         <v>0.8</v>
@@ -1647,7 +1748,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <f>A12+0.2</f>
         <v>1</v>
@@ -1662,7 +1763,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1671,12 +1772,12 @@
         <v>0.79999999999999993</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="2"/>
       <c r="B16" s="4" t="s">
         <v>12</v>
@@ -1690,7 +1791,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
@@ -1712,26 +1813,29 @@
       <c r="H17" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B18" s="1">
-        <f>B$8*(((D6-A$9)*(D6-A$10)*(D6-A$11)*(D6-A$12)*(D6-A$13))/((A$8-A$9)*(A$8-A$10)*(A$8-A$11)*(A$8-A$12)*(A$8-A$13)))</f>
+        <f t="shared" ref="B18:B26" si="3">B$8*(((D6-A$9)*(D6-A$10)*(D6-A$11)*(D6-A$12)*(D6-A$13))/((A$8-A$9)*(A$8-A$10)*(A$8-A$11)*(A$8-A$12)*(A$8-A$13)))</f>
         <v>-0.91173391478696508</v>
       </c>
       <c r="C18" s="1">
-        <f>B$9*(((D6-A$8)*(D6-A$10)*(D6-A$11)*(D6-A$12)*(D6-A$13))/((A$9-A$8)*(A$9-A$10)*(A$9-A$11)*(A$9-A$12)*(A$9-A$13)))</f>
+        <f t="shared" ref="C18:C26" si="4">B$9*(((D6-A$8)*(D6-A$10)*(D6-A$11)*(D6-A$12)*(D6-A$13))/((A$9-A$8)*(A$9-A$10)*(A$9-A$11)*(A$9-A$12)*(A$9-A$13)))</f>
         <v>0</v>
       </c>
       <c r="D18" s="1">
-        <f>B$10*(((D6-A$8)*(D6-A$9)*(D6-A$11)*(D6-A$12)*(D6-A$13))/((A$10-A$8)*(A$10-A$9)*(A$10-A$11)*(A$10-A$12)*(A$10-A$13)))</f>
+        <f t="shared" ref="D18:D26" si="5">B$10*(((D6-A$8)*(D6-A$9)*(D6-A$11)*(D6-A$12)*(D6-A$13))/((A$10-A$8)*(A$10-A$9)*(A$10-A$11)*(A$10-A$12)*(A$10-A$13)))</f>
         <v>0</v>
       </c>
       <c r="E18" s="1">
-        <f>B$11*(((D6-A$8)*(D6-A$9)*(D6-A$10)*(D6-A$12)*(D6-A$13))/(($A$11-$A$8)*($A$11-$A$9)*($A$11-$A$10)*($A$11-$A$12)*($A$11-$A$13)))</f>
+        <f t="shared" ref="E18:E26" si="6">B$11*(((D6-A$8)*(D6-A$9)*(D6-A$10)*(D6-A$12)*(D6-A$13))/(($A$11-$A$8)*($A$11-$A$9)*($A$11-$A$10)*($A$11-$A$12)*($A$11-$A$13)))</f>
         <v>0</v>
       </c>
       <c r="F18" s="1">
-        <f>$B$12*(((D6-$A$8)*(D6-$A$9)*(D6-$A$10)*(D6-$A$11)*(D6-$A$13))/(($A$12-$A$8)*($A$12-$A$9)*($A$12-$A$10)*($A$12-$A$11)*($A$12-$A$13)))</f>
+        <f t="shared" ref="F18:F26" si="7">$B$12*(((D6-$A$8)*(D6-$A$9)*(D6-$A$10)*(D6-$A$11)*(D6-$A$13))/(($A$12-$A$8)*($A$12-$A$9)*($A$12-$A$10)*($A$12-$A$11)*($A$12-$A$13)))</f>
         <v>0</v>
       </c>
       <c r="G18" s="1">
@@ -1739,149 +1843,169 @@
         <v>-0.91173391478696508</v>
       </c>
       <c r="H18" s="1">
-        <f>COS(D6+EXP(COS(D6)))</f>
+        <f t="shared" ref="H18:H27" si="8">COS(D6+EXP(COS(D6)))</f>
         <v>-0.91173391478696508</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="1">
+        <f>H$29*(D6^4)+H$30*(D6^3)+H$31*(D6^2)+H$32*D6+H$33*1</f>
+        <v>-0.91169999999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B19" s="1">
-        <f>B$8*(((D7-A$9)*(D7-A$10)*(D7-A$11)*(D7-A$12)*(D7-A$13))/((A$8-A$9)*(A$8-A$10)*(A$8-A$11)*(A$8-A$12)*(A$8-A$13)))</f>
+        <f t="shared" si="3"/>
         <v>-0.22437201809210472</v>
       </c>
       <c r="C19" s="1">
-        <f>B$9*(((D7-A$8)*(D7-A$10)*(D7-A$11)*(D7-A$12)*(D7-A$13))/((A$9-A$8)*(A$9-A$10)*(A$9-A$11)*(A$9-A$12)*(A$9-A$13)))</f>
+        <f t="shared" si="4"/>
         <v>-1.1835772932068949</v>
       </c>
       <c r="D19" s="1">
-        <f>B$10*(((D7-A$8)*(D7-A$9)*(D7-A$11)*(D7-A$12)*(D7-A$13))/((A$10-A$8)*(A$10-A$9)*(A$10-A$11)*(A$10-A$12)*(A$10-A$13)))</f>
+        <f t="shared" si="5"/>
         <v>0.79877826596347701</v>
       </c>
       <c r="E19" s="1">
-        <f>B$11*(((D7-A$8)*(D7-A$9)*(D7-A$10)*(D7-A$12)*(D7-A$13))/(($A$11-$A$8)*($A$11-$A$9)*($A$11-$A$10)*($A$11-$A$12)*($A$11-$A$13)))</f>
+        <f t="shared" si="6"/>
         <v>-0.47577817695061075</v>
       </c>
       <c r="F19" s="1">
-        <f>$B$12*(((D7-$A$8)*(D7-$A$9)*(D7-$A$10)*(D7-$A$11)*(D7-$A$13))/(($A$12-$A$8)*($A$12-$A$9)*($A$12-$A$10)*($A$12-$A$11)*($A$12-$A$13)))</f>
+        <f t="shared" si="7"/>
         <v>0.16604075536998958</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" ref="G19:G22" si="3">SUM(B19:F19)</f>
+        <f t="shared" ref="G19:G22" si="9">SUM(B19:F19)</f>
         <v>-0.91890846691614381</v>
       </c>
       <c r="H19" s="1">
-        <f>COS(D7+EXP(COS(D7)))</f>
+        <f t="shared" si="8"/>
         <v>-0.94379814193779332</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="1">
+        <f t="shared" ref="I19:I27" si="10">H$29*(D7^4)+H$30*(D7^3)+H$31*(D7^2)+H$32*D7+H$33*1</f>
+        <v>-0.94344609374999999</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B20" s="1">
-        <f>B$8*(((D8-A$9)*(D8-A$10)*(D8-A$11)*(D8-A$12)*(D8-A$13))/((A$8-A$9)*(A$8-A$10)*(A$8-A$11)*(A$8-A$12)*(A$8-A$13)))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="C20" s="1">
-        <f>B$9*(((D8-A$8)*(D8-A$10)*(D8-A$11)*(D8-A$12)*(D8-A$13))/((A$9-A$8)*(A$9-A$10)*(A$9-A$11)*(A$9-A$12)*(A$9-A$13)))</f>
+        <f t="shared" si="4"/>
         <v>-0.96189138749512737</v>
       </c>
       <c r="D20" s="1">
-        <f>B$10*(((D8-A$8)*(D8-A$9)*(D8-A$11)*(D8-A$12)*(D8-A$13))/((A$10-A$8)*(A$10-A$9)*(A$10-A$11)*(A$10-A$12)*(A$10-A$13)))</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="E20" s="1">
-        <f>B$11*(((D8-A$8)*(D8-A$9)*(D8-A$10)*(D8-A$12)*(D8-A$13))/(($A$11-$A$8)*($A$11-$A$9)*($A$11-$A$10)*($A$11-$A$12)*($A$11-$A$13)))</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F20" s="1">
-        <f>$B$12*(((D8-$A$8)*(D8-$A$9)*(D8-$A$10)*(D8-$A$11)*(D8-$A$13))/(($A$12-$A$8)*($A$12-$A$9)*($A$12-$A$10)*($A$12-$A$11)*($A$12-$A$13)))</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G20" s="1">
+        <f t="shared" si="9"/>
+        <v>-0.96189138749512737</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="8"/>
+        <v>-0.96189138749512737</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" si="10"/>
+        <v>-0.96189999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B21" s="1">
         <f t="shared" si="3"/>
-        <v>-0.96189138749512737</v>
-      </c>
-      <c r="H20" s="1">
-        <f>COS(D8+EXP(COS(D8)))</f>
-        <v>-0.96189138749512737</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="1">
-        <f>B$8*(((D9-A$9)*(D9-A$10)*(D9-A$11)*(D9-A$12)*(D9-A$13))/((A$8-A$9)*(A$8-A$10)*(A$8-A$11)*(A$8-A$12)*(A$8-A$13)))</f>
         <v>2.4930224232456069E-2</v>
       </c>
       <c r="C21" s="1">
-        <f>B$9*(((D9-A$8)*(D9-A$10)*(D9-A$11)*(D9-A$12)*(D9-A$13))/((A$9-A$8)*(A$9-A$10)*(A$9-A$11)*(A$9-A$12)*(A$9-A$13)))</f>
+        <f t="shared" si="4"/>
         <v>-0.39452576440229808</v>
       </c>
       <c r="D21" s="1">
-        <f>B$10*(((D9-A$8)*(D9-A$9)*(D9-A$11)*(D9-A$12)*(D9-A$13))/((A$10-A$8)*(A$10-A$9)*(A$10-A$11)*(A$10-A$12)*(A$10-A$13)))</f>
+        <f t="shared" si="5"/>
         <v>-0.7987782659634769</v>
       </c>
       <c r="E21" s="1">
-        <f>B$11*(((D9-A$8)*(D9-A$9)*(D9-A$10)*(D9-A$12)*(D9-A$13))/(($A$11-$A$8)*($A$11-$A$9)*($A$11-$A$10)*($A$11-$A$12)*($A$11-$A$13)))</f>
+        <f t="shared" si="6"/>
         <v>0.26432120941700588</v>
       </c>
       <c r="F21" s="1">
-        <f>$B$12*(((D9-$A$8)*(D9-$A$9)*(D9-$A$10)*(D9-$A$11)*(D9-$A$13))/(($A$12-$A$8)*($A$12-$A$9)*($A$12-$A$10)*($A$12-$A$11)*($A$12-$A$13)))</f>
+        <f t="shared" si="7"/>
         <v>-7.7485685839328425E-2</v>
       </c>
       <c r="G21" s="1">
+        <f t="shared" si="9"/>
+        <v>-0.98153828255564146</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="8"/>
+        <v>-0.97084924322141375</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" si="10"/>
+        <v>-0.97100234374999994</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B22" s="1">
         <f t="shared" si="3"/>
-        <v>-0.98153828255564146</v>
-      </c>
-      <c r="H21" s="1">
-        <f>COS(D9+EXP(COS(D9)))</f>
-        <v>-0.97084924322141375</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="1">
-        <f>B$8*(((D10-A$9)*(D10-A$10)*(D10-A$11)*(D10-A$12)*(D10-A$13))/((A$8-A$9)*(A$8-A$10)*(A$8-A$11)*(A$8-A$12)*(A$8-A$13)))</f>
         <v>0</v>
       </c>
       <c r="C22" s="1">
-        <f>B$9*(((D10-A$8)*(D10-A$10)*(D10-A$11)*(D10-A$12)*(D10-A$13))/((A$9-A$8)*(A$9-A$10)*(A$9-A$11)*(A$9-A$12)*(A$9-A$13)))</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D22" s="1">
-        <f>B$10*(((D10-A$8)*(D10-A$9)*(D10-A$11)*(D10-A$12)*(D10-A$13))/((A$10-A$8)*(A$10-A$9)*(A$10-A$11)*(A$10-A$12)*(A$10-A$13)))</f>
+        <f t="shared" si="5"/>
         <v>-0.97374874326976235</v>
       </c>
       <c r="E22" s="1">
-        <f>B$11*(((D10-A$8)*(D10-A$9)*(D10-A$10)*(D10-A$12)*(D10-A$13))/(($A$11-$A$8)*($A$11-$A$9)*($A$11-$A$10)*($A$11-$A$12)*($A$11-$A$13)))</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F22" s="1">
-        <f>$B$12*(((D10-$A$8)*(D10-$A$9)*(D10-$A$10)*(D10-$A$11)*(D10-$A$13))/(($A$12-$A$8)*($A$12-$A$9)*($A$12-$A$10)*($A$12-$A$11)*($A$12-$A$13)))</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G22" s="1">
+        <f t="shared" si="9"/>
+        <v>-0.97374874326976235</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="8"/>
+        <v>-0.97374874326976235</v>
+      </c>
+      <c r="I22" s="1">
+        <f t="shared" si="10"/>
+        <v>-0.97370000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B23" s="1">
         <f t="shared" si="3"/>
-        <v>-0.97374874326976235</v>
-      </c>
-      <c r="H22" s="1">
-        <f>COS(D10+EXP(COS(D10)))</f>
-        <v>-0.97374874326976235</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="1">
-        <f>B$8*(((D11-A$9)*(D11-A$10)*(D11-A$11)*(D11-A$12)*(D11-A$13))/((A$8-A$9)*(A$8-A$10)*(A$8-A$11)*(A$8-A$12)*(A$8-A$13)))</f>
         <v>-1.068438181390975E-2</v>
       </c>
       <c r="C23" s="1">
-        <f>B$9*(((D11-A$8)*(D11-A$10)*(D11-A$11)*(D11-A$12)*(D11-A$13))/((A$9-A$8)*(A$9-A$10)*(A$9-A$11)*(A$9-A$12)*(A$9-A$13)))</f>
+        <f t="shared" si="4"/>
         <v>9.3934705810071045E-2</v>
       </c>
       <c r="D23" s="1">
-        <f>B$10*(((D11-A$8)*(D11-A$9)*(D11-A$11)*(D11-A$12)*(D11-A$13))/((A$10-A$8)*(A$10-A$9)*(A$10-A$11)*(A$10-A$12)*(A$10-A$13)))</f>
+        <f t="shared" si="5"/>
         <v>-0.57055590425962677</v>
       </c>
       <c r="E23" s="1">
-        <f>B$11*(((D11-A$8)*(D11-A$9)*(D11-A$10)*(D11-A$12)*(D11-A$13))/(($A$11-$A$8)*($A$11-$A$9)*($A$11-$A$10)*($A$11-$A$12)*($A$11-$A$13)))</f>
+        <f t="shared" si="6"/>
         <v>-0.56640259160786965</v>
       </c>
       <c r="F23" s="1">
-        <f>$B$12*(((D11-$A$8)*(D11-$A$9)*(D11-$A$10)*(D11-$A$11)*(D11-$A$13))/(($A$12-$A$8)*($A$12-$A$9)*($A$12-$A$10)*($A$12-$A$11)*($A$12-$A$13)))</f>
+        <f t="shared" si="7"/>
         <v>9.2244864094438647E-2</v>
       </c>
       <c r="G23" s="1">
@@ -1889,89 +2013,101 @@
         <v>-0.96146330777689659</v>
       </c>
       <c r="H23" s="1">
-        <f>COS(D11+EXP(COS(D11)))</f>
+        <f t="shared" si="8"/>
         <v>-0.97216067704633868</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="1">
+        <f t="shared" si="10"/>
+        <v>-0.97194609374999996</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B24" s="1">
-        <f>B$8*(((D12-A$9)*(D12-A$10)*(D12-A$11)*(D12-A$12)*(D12-A$13))/((A$8-A$9)*(A$8-A$10)*(A$8-A$11)*(A$8-A$12)*(A$8-A$13)))</f>
+        <f t="shared" si="3"/>
         <v>-1.687046640880198E-17</v>
       </c>
       <c r="C24" s="1">
-        <f>B$9*(((D12-A$8)*(D12-A$10)*(D12-A$11)*(D12-A$12)*(D12-A$13))/((A$9-A$8)*(A$9-A$10)*(A$9-A$11)*(A$9-A$12)*(A$9-A$13)))</f>
+        <f t="shared" si="4"/>
         <v>1.3348924569821602E-16</v>
       </c>
       <c r="D24" s="1">
-        <f>B$10*(((D12-A$8)*(D12-A$9)*(D12-A$11)*(D12-A$12)*(D12-A$13))/((A$10-A$8)*(A$10-A$9)*(A$10-A$11)*(A$10-A$12)*(A$10-A$13)))</f>
+        <f t="shared" si="5"/>
         <v>-5.4053913748895019E-16</v>
       </c>
       <c r="E24" s="1">
-        <f>B$11*(((D12-A$8)*(D12-A$9)*(D12-A$10)*(D12-A$12)*(D12-A$13))/(($A$11-$A$8)*($A$11-$A$9)*($A$11-$A$10)*($A$11-$A$12)*($A$11-$A$13)))</f>
+        <f t="shared" si="6"/>
         <v>-0.96666042301076427</v>
       </c>
       <c r="F24" s="1">
-        <f>$B$12*(((D12-$A$8)*(D12-$A$9)*(D12-$A$10)*(D12-$A$11)*(D12-$A$13))/(($A$12-$A$8)*($A$12-$A$9)*($A$12-$A$10)*($A$12-$A$11)*($A$12-$A$13)))</f>
+        <f t="shared" si="7"/>
         <v>2.6217567237392405E-16</v>
       </c>
       <c r="G24" s="1">
-        <f t="shared" ref="G24:G25" si="4">SUM(B24:F24)</f>
+        <f t="shared" ref="G24:G25" si="11">SUM(B24:F24)</f>
         <v>-0.96666042301076449</v>
       </c>
       <c r="H24" s="1">
-        <f>COS(D12+EXP(COS(D12)))</f>
+        <f t="shared" si="8"/>
         <v>-0.9666604230107646</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="1">
+        <f t="shared" si="10"/>
+        <v>-0.96669999999999989</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B25" s="1">
-        <f>B$8*(((D13-A$9)*(D13-A$10)*(D13-A$11)*(D13-A$12)*(D13-A$13))/((A$8-A$9)*(A$8-A$10)*(A$8-A$11)*(A$8-A$12)*(A$8-A$13)))</f>
+        <f t="shared" si="3"/>
         <v>1.0684381813909734E-2</v>
       </c>
       <c r="C25" s="1">
-        <f>B$9*(((D13-A$8)*(D13-A$10)*(D13-A$11)*(D13-A$12)*(D13-A$13))/((A$9-A$8)*(A$9-A$10)*(A$9-A$11)*(A$9-A$12)*(A$9-A$13)))</f>
+        <f t="shared" si="4"/>
         <v>-7.8905152880459573E-2</v>
       </c>
       <c r="D25" s="1">
-        <f>B$10*(((D13-A$8)*(D13-A$9)*(D13-A$11)*(D13-A$12)*(D13-A$13))/((A$10-A$8)*(A$10-A$9)*(A$10-A$11)*(A$10-A$12)*(A$10-A$13)))</f>
+        <f t="shared" si="5"/>
         <v>0.26625942198782543</v>
       </c>
       <c r="E25" s="1">
-        <f>B$11*(((D13-A$8)*(D13-A$9)*(D13-A$10)*(D13-A$12)*(D13-A$13))/(($A$11-$A$8)*($A$11-$A$9)*($A$11-$A$10)*($A$11-$A$12)*($A$11-$A$13)))</f>
+        <f t="shared" si="6"/>
         <v>-0.79296362825101807</v>
       </c>
       <c r="F25" s="1">
-        <f>$B$12*(((D13-$A$8)*(D13-$A$9)*(D13-$A$10)*(D13-$A$11)*(D13-$A$13))/(($A$12-$A$8)*($A$12-$A$9)*($A$12-$A$10)*($A$12-$A$11)*($A$12-$A$13)))</f>
+        <f t="shared" si="7"/>
         <v>-0.38742842919664139</v>
       </c>
       <c r="G25" s="1">
+        <f t="shared" si="11"/>
+        <v>-0.98235340652638392</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="8"/>
+        <v>-0.95739978929344105</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" si="10"/>
+        <v>-0.95792734374999988</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B26" s="1">
+        <f t="shared" si="3"/>
+        <v>2.5305699613202941E-17</v>
+      </c>
+      <c r="C26" s="1">
         <f t="shared" si="4"/>
-        <v>-0.98235340652638392</v>
-      </c>
-      <c r="H25" s="1">
-        <f>COS(D13+EXP(COS(D13)))</f>
-        <v>-0.95739978929344105</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="1">
-        <f>B$8*(((D14-A$9)*(D14-A$10)*(D14-A$11)*(D14-A$12)*(D14-A$13))/((A$8-A$9)*(A$8-A$10)*(A$8-A$11)*(A$8-A$12)*(A$8-A$13)))</f>
-        <v>2.5305699613202941E-17</v>
-      </c>
-      <c r="C26" s="1">
-        <f>B$9*(((D14-A$8)*(D14-A$10)*(D14-A$11)*(D14-A$12)*(D14-A$13))/((A$9-A$8)*(A$9-A$10)*(A$9-A$11)*(A$9-A$12)*(A$9-A$13)))</f>
         <v>-1.7798566093095455E-16</v>
       </c>
       <c r="D26" s="1">
-        <f>B$10*(((D14-A$8)*(D14-A$9)*(D14-A$11)*(D14-A$12)*(D14-A$13))/((A$10-A$8)*(A$10-A$9)*(A$10-A$11)*(A$10-A$12)*(A$10-A$13)))</f>
+        <f t="shared" si="5"/>
         <v>5.405391374889497E-16</v>
       </c>
       <c r="E26" s="1">
-        <f>B$11*(((D14-A$8)*(D14-A$9)*(D14-A$10)*(D14-A$12)*(D14-A$13))/(($A$11-$A$8)*($A$11-$A$9)*($A$11-$A$10)*($A$11-$A$12)*($A$11-$A$13)))</f>
+        <f t="shared" si="6"/>
         <v>-1.0732086586204438E-15</v>
       </c>
       <c r="F26" s="1">
-        <f>$B$12*(((D14-$A$8)*(D14-$A$9)*(D14-$A$10)*(D14-$A$11)*(D14-$A$13))/(($A$12-$A$8)*($A$12-$A$9)*($A$12-$A$10)*($A$12-$A$11)*($A$12-$A$13)))</f>
+        <f t="shared" si="7"/>
         <v>-0.94458740832705013</v>
       </c>
       <c r="G26" s="1">
@@ -1979,11 +2115,15 @@
         <v>-0.94458740832705079</v>
       </c>
       <c r="H26" s="1">
-        <f>COS(D14+EXP(COS(D14)))</f>
+        <f t="shared" si="8"/>
         <v>-0.94458740832705113</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="1">
+        <f t="shared" si="10"/>
+        <v>-0.9446</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.45">
       <c r="B27" s="1">
         <f>B$8*(((E15-A$9)*(E15-A$10)*(E15-A$11)*(E15-A$12)*(E15-A$13))/((A$8-A$9)*(A$8-A$10)*(A$8-A$11)*(A$8-A$12)*(A$8-A$13)))</f>
         <v>-0.91173391478696508</v>
@@ -2005,18 +2145,102 @@
         <v>0</v>
       </c>
       <c r="G27" s="1">
-        <f t="shared" ref="G27" si="5">SUM(B27:F27)</f>
+        <f t="shared" ref="G27" si="12">SUM(B27:F27)</f>
         <v>-0.91173391478696508</v>
       </c>
       <c r="H27" s="1">
-        <f>COS(D15+EXP(COS(D15)))</f>
+        <f t="shared" si="8"/>
         <v>-0.91173391478696508</v>
       </c>
+      <c r="I27" s="1">
+        <f t="shared" si="10"/>
+        <v>-0.91169999999999995</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="G29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H29" s="1">
+        <f>99375/240000</f>
+        <v>0.4140625</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B30" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="G30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H30" s="1">
+        <f>-217250/240000</f>
+        <v>-0.90520833333333328</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B31" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="G31" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H31" s="1">
+        <f>217725/240000</f>
+        <v>0.90718750000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B32" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="G32" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H32" s="1">
+        <f>-95890/240000</f>
+        <v>-0.39954166666666668</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="B33" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="G33" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H33" s="1">
+        <f>-218808/240000</f>
+        <v>-0.91169999999999995</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="7">
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B33:E33"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="B31:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2031,23 +2255,23 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.73046875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.3984375" customWidth="1"/>
+    <col min="5" max="5" width="12.73046875" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -2061,7 +2285,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2075,7 +2299,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
@@ -2089,7 +2313,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -2115,7 +2339,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -2147,7 +2371,7 @@
         <v>-1.0750080124661276E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <f>A8+0.1</f>
         <v>4.0999999999999996</v>
@@ -2178,7 +2402,7 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <f t="shared" ref="A10:A12" si="3">A9+0.1</f>
         <v>4.1999999999999993</v>
@@ -2206,7 +2430,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <f t="shared" si="3"/>
         <v>4.2999999999999989</v>
@@ -2231,7 +2455,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <f t="shared" si="3"/>
         <v>4.3999999999999986</v>
@@ -2253,7 +2477,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="D14" s="1" t="s">
         <v>15</v>
       </c>
@@ -2267,7 +2491,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="D15" s="1">
         <f>D8</f>
         <v>4</v>
@@ -2285,19 +2509,19 @@
         <v>3.9000000000000106</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D17" s="4" t="s">
         <v>27</v>
       </c>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.45">
       <c r="D18" s="1" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
feat: math hw5 completed
</commit_message>
<xml_diff>
--- a/Математика/ДЗ_5.xlsx
+++ b/Математика/ДЗ_5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tony_\OneDrive\Документы\omstu-works-2\Математика\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\omstu-works-2\Математика\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396F5D0C-D2B6-41AB-AB86-CCF36A522F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1EE215-3EDA-4418-9EF6-BD275EFF1828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Многочлен Лагранжа" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
   <si>
     <t>Вариант 26</t>
   </si>
@@ -52,9 +52,6 @@
     <t>y</t>
   </si>
   <si>
-    <t>L</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -155,6 +152,36 @@
   </si>
   <si>
     <t>L сокращенный</t>
+  </si>
+  <si>
+    <t>Проверка</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>L полный</t>
+  </si>
+  <si>
+    <t>Первая производная по формуле Ньютона</t>
+  </si>
+  <si>
+    <t>f'(4)</t>
+  </si>
+  <si>
+    <t>-sin(x+e^(cos(x)))*(1-sin(x)*e^(cos(x)))</t>
+  </si>
+  <si>
+    <t>Вторая производная по формуле Ньютона</t>
+  </si>
+  <si>
+    <t>f'(4,4)</t>
+  </si>
+  <si>
+    <t>-cos(x+e^(cos(x)))*((1-sin(x)*e^(cos(x)))^2)-sin(x+e^(cos(x)))*e^(cos(x))*(sin^2(x)-cos(x))</t>
+  </si>
+  <si>
+    <t>delta</t>
   </si>
 </sst>
 </file>
@@ -231,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -245,6 +272,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -327,7 +355,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -357,75 +385,48 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Многочлен Лагранжа'!$D$6:$D$14</c:f>
+              <c:f>'Многочлен Лагранжа'!$A$18:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.2</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.30000000000000004</c:v>
+                  <c:v>0.60000000000000009</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.79999999999999993</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Многочлен Лагранжа'!$H$18:$H$27</c:f>
+              <c:f>'Многочлен Лагранжа'!$I$18:$I$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>-0.91173391478696508</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.94379814193779332</c:v>
+                  <c:v>-0.96189138749512737</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.96189138749512737</c:v>
+                  <c:v>-0.97374874326976235</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.97084924322141375</c:v>
+                  <c:v>-0.9666604230107646</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.97374874326976235</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-0.97216067704633868</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-0.9666604230107646</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-0.95739978929344105</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-0.94458740832705113</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-0.91173391478696508</c:v>
+                  <c:v>-0.94458740832705101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -457,75 +458,48 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Многочлен Лагранжа'!$D$6:$D$14</c:f>
+              <c:f>'Многочлен Лагранжа'!$A$18:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.2</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.30000000000000004</c:v>
+                  <c:v>0.60000000000000009</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.79999999999999993</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Многочлен Лагранжа'!$G$18:$G$27</c:f>
+              <c:f>'Многочлен Лагранжа'!$G$18:$G$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>-0.91173391478696508</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.91890846691614381</c:v>
+                  <c:v>-0.96189138749512737</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.96189138749512737</c:v>
+                  <c:v>-0.97374874326976235</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.98153828255564146</c:v>
+                  <c:v>-0.9666604230107646</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.97374874326976235</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-0.96146330777689659</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-0.96666042301076449</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-0.98235340652638392</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-0.94458740832705079</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-0.91173391478696508</c:v>
+                  <c:v>-0.94458740832705101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -555,41 +529,50 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Многочлен Лагранжа'!$A$18:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.60000000000000009</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Многочлен Лагранжа'!$I$18:$I$27</c:f>
+              <c:f>'Многочлен Лагранжа'!$H$18:$H$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>-0.91169999999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.94344609374999999</c:v>
+                  <c:v>-0.96189999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.96189999999999998</c:v>
+                  <c:v>-0.97370000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.97100234374999994</c:v>
+                  <c:v>-0.96669999999999989</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.97370000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-0.97194609374999996</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-0.96669999999999989</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-0.95792734374999988</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-0.9446</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-0.91169999999999995</c:v>
+                  <c:v>-0.94459999999999988</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -654,7 +637,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2033121040"/>
@@ -713,7 +696,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2033120208"/>
@@ -754,7 +737,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="ru-RU"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1625,60 +1608,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="D5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="1">
-        <f>D6+0.1</f>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -1686,156 +1657,134 @@
         <f>COS(A8+EXP(COS(A8)))</f>
         <v>-0.91173391478696508</v>
       </c>
-      <c r="D8" s="1">
-        <f t="shared" ref="D8:D13" si="0">D7+0.1</f>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f>A8+0.2</f>
         <v>0.2</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" ref="B9:B13" si="1">COS(A9+EXP(COS(A9)))</f>
+        <f t="shared" ref="B9:B13" si="0">COS(A9+EXP(COS(A9)))</f>
         <v>-0.96189138749512737</v>
       </c>
-      <c r="D9" s="1">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <f t="shared" ref="A10:A12" si="1">A9+0.2</f>
+        <v>0.4</v>
+      </c>
+      <c r="B10" s="1">
         <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A10" s="1">
-        <f t="shared" ref="A10:A12" si="2">A9+0.2</f>
-        <v>0.4</v>
-      </c>
-      <c r="B10" s="1">
+        <v>-0.97374874326976235</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <f t="shared" si="1"/>
-        <v>-0.97374874326976235</v>
-      </c>
-      <c r="D10" s="1">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="B11" s="1">
         <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A11" s="1">
-        <f t="shared" si="2"/>
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="B11" s="1">
+        <v>-0.9666604230107646</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <f t="shared" si="1"/>
-        <v>-0.9666604230107646</v>
-      </c>
-      <c r="D11" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="B12" s="1">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" s="1">
-        <f t="shared" si="2"/>
-        <v>0.8</v>
-      </c>
-      <c r="B12" s="1">
-        <f t="shared" si="1"/>
         <v>-0.94458740832705101</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="1">
-        <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f>A12+0.2</f>
         <v>1</v>
       </c>
       <c r="B13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-0.91101112436955167</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="1">
-        <f t="shared" si="0"/>
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="1">
-        <f>D13+0.1</f>
-        <v>0.79999999999999993</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A16" s="2"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
       <c r="B16" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="H16" s="4"/>
+      <c r="I16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="G17" s="3" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="H17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I17" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>0</v>
+      </c>
       <c r="B18" s="1">
-        <f t="shared" ref="B18:B26" si="3">B$8*(((D6-A$9)*(D6-A$10)*(D6-A$11)*(D6-A$12)*(D6-A$13))/((A$8-A$9)*(A$8-A$10)*(A$8-A$11)*(A$8-A$12)*(A$8-A$13)))</f>
+        <f>B$8*(((A18-A$9)*(A18-A$10)*(A18-A$11)*(A18-A$12)*(A18-A$13))/((A$8-A$9)*(A$8-A$10)*(A$8-A$11)*(A$8-A$12)*(A$8-A$13)))</f>
         <v>-0.91173391478696508</v>
       </c>
-      <c r="C18" s="1">
-        <f t="shared" ref="C18:C26" si="4">B$9*(((D6-A$8)*(D6-A$10)*(D6-A$11)*(D6-A$12)*(D6-A$13))/((A$9-A$8)*(A$9-A$10)*(A$9-A$11)*(A$9-A$12)*(A$9-A$13)))</f>
+      <c r="C18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="1">
+        <f>B$10*(((A18-A$8)*(A18-A$9)*(A18-A$11)*(A18-A$12)*(A18-A$13))/((A$10-A$8)*(A$10-A$9)*(A$10-A$11)*(A$10-A$12)*(A$10-A$13)))</f>
         <v>0</v>
       </c>
-      <c r="D18" s="1">
-        <f t="shared" ref="D18:D26" si="5">B$10*(((D6-A$8)*(D6-A$9)*(D6-A$11)*(D6-A$12)*(D6-A$13))/((A$10-A$8)*(A$10-A$9)*(A$10-A$11)*(A$10-A$12)*(A$10-A$13)))</f>
+      <c r="E18" s="1">
+        <f>B$11*(((A18-A$8)*(A18-A$9)*(A18-A$10)*(A18-A$12)*(A18-A$13))/(($A$11-$A$8)*($A$11-$A$9)*($A$11-$A$10)*($A$11-$A$12)*($A$11-$A$13)))</f>
         <v>0</v>
       </c>
-      <c r="E18" s="1">
-        <f t="shared" ref="E18:E26" si="6">B$11*(((D6-A$8)*(D6-A$9)*(D6-A$10)*(D6-A$12)*(D6-A$13))/(($A$11-$A$8)*($A$11-$A$9)*($A$11-$A$10)*($A$11-$A$12)*($A$11-$A$13)))</f>
-        <v>0</v>
-      </c>
       <c r="F18" s="1">
-        <f t="shared" ref="F18:F26" si="7">$B$12*(((D6-$A$8)*(D6-$A$9)*(D6-$A$10)*(D6-$A$11)*(D6-$A$13))/(($A$12-$A$8)*($A$12-$A$9)*($A$12-$A$10)*($A$12-$A$11)*($A$12-$A$13)))</f>
+        <f>$B$12*(((A18-$A$8)*(A18-$A$9)*(A18-$A$10)*(A18-$A$11)*(A18-$A$13))/(($A$12-$A$8)*($A$12-$A$9)*($A$12-$A$10)*($A$12-$A$11)*($A$12-$A$13)))</f>
         <v>0</v>
       </c>
       <c r="G18" s="1">
@@ -1843,404 +1792,250 @@
         <v>-0.91173391478696508</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" ref="H18:H27" si="8">COS(D6+EXP(COS(D6)))</f>
+        <f>H$24*(A18^4)+H$25*(A18^3)+H$26*(A18^2)+H$27*A18+H$28*1</f>
+        <v>-0.91169999999999995</v>
+      </c>
+      <c r="I18" s="1">
+        <f>COS(A18+EXP(COS(A18)))</f>
         <v>-0.91173391478696508</v>
       </c>
-      <c r="I18" s="1">
-        <f>H$29*(D6^4)+H$30*(D6^3)+H$31*(D6^2)+H$32*D6+H$33*1</f>
-        <v>-0.91169999999999995</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <f>A18+0.2</f>
+        <v>0.2</v>
+      </c>
       <c r="B19" s="1">
-        <f t="shared" si="3"/>
-        <v>-0.22437201809210472</v>
+        <f>B$8*(((A19-A$9)*(A19-A$10)*(A19-A$11)*(A19-A$12)*(A19-A$13))/((A$8-A$9)*(A$8-A$10)*(A$8-A$11)*(A$8-A$12)*(A$8-A$13)))</f>
+        <v>0</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" si="4"/>
-        <v>-1.1835772932068949</v>
+        <f>B$9*(((A19-A$8)*(A19-A$10)*(A19-A$11)*(A19-A$12)*(A19-A$13))/((A$9-A$8)*(A$9-A$10)*(A$9-A$11)*(A$9-A$12)*(A$9-A$13)))</f>
+        <v>-0.96189138749512737</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="5"/>
-        <v>0.79877826596347701</v>
+        <f>B$10*(((A19-A$8)*(A19-A$9)*(A19-A$11)*(A19-A$12)*(A19-A$13))/((A$10-A$8)*(A$10-A$9)*(A$10-A$11)*(A$10-A$12)*(A$10-A$13)))</f>
+        <v>0</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="6"/>
-        <v>-0.47577817695061075</v>
+        <f>B$11*(((A19-A$8)*(A19-A$9)*(A19-A$10)*(A19-A$12)*(A19-A$13))/(($A$11-$A$8)*($A$11-$A$9)*($A$11-$A$10)*($A$11-$A$12)*($A$11-$A$13)))</f>
+        <v>0</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="7"/>
-        <v>0.16604075536998958</v>
+        <f>$B$12*(((A19-$A$8)*(A19-$A$9)*(A19-$A$10)*(A19-$A$11)*(A19-$A$13))/(($A$12-$A$8)*($A$12-$A$9)*($A$12-$A$10)*($A$12-$A$11)*($A$12-$A$13)))</f>
+        <v>0</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" ref="G19:G22" si="9">SUM(B19:F19)</f>
-        <v>-0.91890846691614381</v>
+        <f t="shared" ref="G19:G22" si="2">SUM(B19:F19)</f>
+        <v>-0.96189138749512737</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" si="8"/>
-        <v>-0.94379814193779332</v>
+        <f>H$24*(A19^4)+H$25*(A19^3)+H$26*(A19^2)+H$27*A19+H$28*1</f>
+        <v>-0.96189999999999998</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" ref="I19:I27" si="10">H$29*(D7^4)+H$30*(D7^3)+H$31*(D7^2)+H$32*D7+H$33*1</f>
-        <v>-0.94344609374999999</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.45">
+        <f>COS(A19+EXP(COS(A19)))</f>
+        <v>-0.96189138749512737</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <f>A19+0.2</f>
+        <v>0.4</v>
+      </c>
       <c r="B20" s="1">
-        <f t="shared" si="3"/>
+        <f>B$8*(((A20-A$9)*(A20-A$10)*(A20-A$11)*(A20-A$12)*(A20-A$13))/((A$8-A$9)*(A$8-A$10)*(A$8-A$11)*(A$8-A$12)*(A$8-A$13)))</f>
         <v>0</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" si="4"/>
-        <v>-0.96189138749512737</v>
+        <f>B$9*(((A20-A$8)*(A20-A$10)*(A20-A$11)*(A20-A$12)*(A20-A$13))/((A$9-A$8)*(A$9-A$10)*(A$9-A$11)*(A$9-A$12)*(A$9-A$13)))</f>
+        <v>0</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="5"/>
+        <f>B$10*(((A20-A$8)*(A20-A$9)*(A20-A$11)*(A20-A$12)*(A20-A$13))/((A$10-A$8)*(A$10-A$9)*(A$10-A$11)*(A$10-A$12)*(A$10-A$13)))</f>
+        <v>-0.97374874326976235</v>
+      </c>
+      <c r="E20" s="1">
+        <f>B$11*(((A20-A$8)*(A20-A$9)*(A20-A$10)*(A20-A$12)*(A20-A$13))/(($A$11-$A$8)*($A$11-$A$9)*($A$11-$A$10)*($A$11-$A$12)*($A$11-$A$13)))</f>
         <v>0</v>
       </c>
-      <c r="E20" s="1">
-        <f t="shared" si="6"/>
+      <c r="F20" s="1">
+        <f>$B$12*(((A20-$A$8)*(A20-$A$9)*(A20-$A$10)*(A20-$A$11)*(A20-$A$13))/(($A$12-$A$8)*($A$12-$A$9)*($A$12-$A$10)*($A$12-$A$11)*($A$12-$A$13)))</f>
         <v>0</v>
       </c>
-      <c r="F20" s="1">
-        <f t="shared" si="7"/>
+      <c r="G20" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.97374874326976235</v>
+      </c>
+      <c r="H20" s="1">
+        <f>H$24*(A20^4)+H$25*(A20^3)+H$26*(A20^2)+H$27*A20+H$28*1</f>
+        <v>-0.97370000000000001</v>
+      </c>
+      <c r="I20" s="1">
+        <f>COS(A20+EXP(COS(A20)))</f>
+        <v>-0.97374874326976235</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <f>A20+0.2</f>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="B21" s="1">
+        <f>B$8*(((A21-A$9)*(A21-A$10)*(A21-A$11)*(A21-A$12)*(A21-A$13))/((A$8-A$9)*(A$8-A$10)*(A$8-A$11)*(A$8-A$12)*(A$8-A$13)))</f>
         <v>0</v>
       </c>
-      <c r="G20" s="1">
-        <f t="shared" si="9"/>
-        <v>-0.96189138749512737</v>
-      </c>
-      <c r="H20" s="1">
-        <f t="shared" si="8"/>
-        <v>-0.96189138749512737</v>
-      </c>
-      <c r="I20" s="1">
-        <f t="shared" si="10"/>
-        <v>-0.96189999999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B21" s="1">
-        <f t="shared" si="3"/>
-        <v>2.4930224232456069E-2</v>
-      </c>
       <c r="C21" s="1">
-        <f t="shared" si="4"/>
-        <v>-0.39452576440229808</v>
+        <f>B$9*(((A21-A$8)*(A21-A$10)*(A21-A$11)*(A21-A$12)*(A21-A$13))/((A$9-A$8)*(A$9-A$10)*(A$9-A$11)*(A$9-A$12)*(A$9-A$13)))</f>
+        <v>0</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="5"/>
-        <v>-0.7987782659634769</v>
+        <f>B$10*(((A21-A$8)*(A21-A$9)*(A21-A$11)*(A21-A$12)*(A21-A$13))/((A$10-A$8)*(A$10-A$9)*(A$10-A$11)*(A$10-A$12)*(A$10-A$13)))</f>
+        <v>0</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" si="6"/>
-        <v>0.26432120941700588</v>
+        <f>B$11*(((A21-A$8)*(A21-A$9)*(A21-A$10)*(A21-A$12)*(A21-A$13))/(($A$11-$A$8)*($A$11-$A$9)*($A$11-$A$10)*($A$11-$A$12)*($A$11-$A$13)))</f>
+        <v>-0.9666604230107646</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="7"/>
-        <v>-7.7485685839328425E-2</v>
+        <f>$B$12*(((A21-$A$8)*(A21-$A$9)*(A21-$A$10)*(A21-$A$11)*(A21-$A$13))/(($A$12-$A$8)*($A$12-$A$9)*($A$12-$A$10)*($A$12-$A$11)*($A$12-$A$13)))</f>
+        <v>0</v>
       </c>
       <c r="G21" s="1">
-        <f t="shared" si="9"/>
-        <v>-0.98153828255564146</v>
+        <f t="shared" si="2"/>
+        <v>-0.9666604230107646</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="8"/>
-        <v>-0.97084924322141375</v>
+        <f>H$24*(A21^4)+H$25*(A21^3)+H$26*(A21^2)+H$27*A21+H$28*1</f>
+        <v>-0.96669999999999989</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" si="10"/>
-        <v>-0.97100234374999994</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.45">
+        <f>COS(A21+EXP(COS(A21)))</f>
+        <v>-0.9666604230107646</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <f>A21+0.2</f>
+        <v>0.8</v>
+      </c>
       <c r="B22" s="1">
-        <f t="shared" si="3"/>
+        <f>B$8*(((A22-A$9)*(A22-A$10)*(A22-A$11)*(A22-A$12)*(A22-A$13))/((A$8-A$9)*(A$8-A$10)*(A$8-A$11)*(A$8-A$12)*(A$8-A$13)))</f>
         <v>0</v>
       </c>
       <c r="C22" s="1">
-        <f t="shared" si="4"/>
+        <f>B$9*(((A22-A$8)*(A22-A$10)*(A22-A$11)*(A22-A$12)*(A22-A$13))/((A$9-A$8)*(A$9-A$10)*(A$9-A$11)*(A$9-A$12)*(A$9-A$13)))</f>
         <v>0</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="5"/>
-        <v>-0.97374874326976235</v>
+        <f>B$10*(((A22-A$8)*(A22-A$9)*(A22-A$11)*(A22-A$12)*(A22-A$13))/((A$10-A$8)*(A$10-A$9)*(A$10-A$11)*(A$10-A$12)*(A$10-A$13)))</f>
+        <v>0</v>
       </c>
       <c r="E22" s="1">
-        <f t="shared" si="6"/>
+        <f>B$11*(((A22-A$8)*(A22-A$9)*(A22-A$10)*(A22-A$12)*(A22-A$13))/(($A$11-$A$8)*($A$11-$A$9)*($A$11-$A$10)*($A$11-$A$12)*($A$11-$A$13)))</f>
         <v>0</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f>$B$12*(((A22-$A$8)*(A22-$A$9)*(A22-$A$10)*(A22-$A$11)*(A22-$A$13))/(($A$12-$A$8)*($A$12-$A$9)*($A$12-$A$10)*($A$12-$A$11)*($A$12-$A$13)))</f>
+        <v>-0.94458740832705101</v>
       </c>
       <c r="G22" s="1">
-        <f t="shared" si="9"/>
-        <v>-0.97374874326976235</v>
+        <f t="shared" si="2"/>
+        <v>-0.94458740832705101</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="8"/>
-        <v>-0.97374874326976235</v>
+        <f>H$24*(A22^4)+H$25*(A22^3)+H$26*(A22^2)+H$27*A22+H$28*1</f>
+        <v>-0.94459999999999988</v>
       </c>
       <c r="I22" s="1">
-        <f t="shared" si="10"/>
-        <v>-0.97370000000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B23" s="1">
-        <f t="shared" si="3"/>
-        <v>-1.068438181390975E-2</v>
-      </c>
-      <c r="C23" s="1">
-        <f t="shared" si="4"/>
-        <v>9.3934705810071045E-2</v>
-      </c>
-      <c r="D23" s="1">
-        <f t="shared" si="5"/>
-        <v>-0.57055590425962677</v>
-      </c>
-      <c r="E23" s="1">
-        <f t="shared" si="6"/>
-        <v>-0.56640259160786965</v>
-      </c>
-      <c r="F23" s="1">
-        <f t="shared" si="7"/>
-        <v>9.2244864094438647E-2</v>
-      </c>
-      <c r="G23" s="1">
-        <f>SUM(B23:F23)</f>
-        <v>-0.96146330777689659</v>
-      </c>
-      <c r="H23" s="1">
-        <f t="shared" si="8"/>
-        <v>-0.97216067704633868</v>
-      </c>
-      <c r="I23" s="1">
-        <f t="shared" si="10"/>
-        <v>-0.97194609374999996</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B24" s="1">
-        <f t="shared" si="3"/>
-        <v>-1.687046640880198E-17</v>
-      </c>
-      <c r="C24" s="1">
-        <f t="shared" si="4"/>
-        <v>1.3348924569821602E-16</v>
-      </c>
-      <c r="D24" s="1">
-        <f t="shared" si="5"/>
-        <v>-5.4053913748895019E-16</v>
-      </c>
-      <c r="E24" s="1">
-        <f t="shared" si="6"/>
-        <v>-0.96666042301076427</v>
-      </c>
-      <c r="F24" s="1">
-        <f t="shared" si="7"/>
-        <v>2.6217567237392405E-16</v>
-      </c>
-      <c r="G24" s="1">
-        <f t="shared" ref="G24:G25" si="11">SUM(B24:F24)</f>
-        <v>-0.96666042301076449</v>
+        <f>COS(A22+EXP(COS(A22)))</f>
+        <v>-0.94458740832705101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="G24" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="8"/>
-        <v>-0.9666604230107646</v>
-      </c>
-      <c r="I24" s="1">
-        <f t="shared" si="10"/>
-        <v>-0.96669999999999989</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B25" s="1">
-        <f t="shared" si="3"/>
-        <v>1.0684381813909734E-2</v>
-      </c>
-      <c r="C25" s="1">
-        <f t="shared" si="4"/>
-        <v>-7.8905152880459573E-2</v>
-      </c>
-      <c r="D25" s="1">
-        <f t="shared" si="5"/>
-        <v>0.26625942198782543</v>
-      </c>
-      <c r="E25" s="1">
-        <f t="shared" si="6"/>
-        <v>-0.79296362825101807</v>
-      </c>
-      <c r="F25" s="1">
-        <f t="shared" si="7"/>
-        <v>-0.38742842919664139</v>
-      </c>
-      <c r="G25" s="1">
-        <f t="shared" si="11"/>
-        <v>-0.98235340652638392</v>
-      </c>
-      <c r="H25" s="1">
-        <f t="shared" si="8"/>
-        <v>-0.95739978929344105</v>
-      </c>
-      <c r="I25" s="1">
-        <f t="shared" si="10"/>
-        <v>-0.95792734374999988</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B26" s="1">
-        <f t="shared" si="3"/>
-        <v>2.5305699613202941E-17</v>
-      </c>
-      <c r="C26" s="1">
-        <f t="shared" si="4"/>
-        <v>-1.7798566093095455E-16</v>
-      </c>
-      <c r="D26" s="1">
-        <f t="shared" si="5"/>
-        <v>5.405391374889497E-16</v>
-      </c>
-      <c r="E26" s="1">
-        <f t="shared" si="6"/>
-        <v>-1.0732086586204438E-15</v>
-      </c>
-      <c r="F26" s="1">
-        <f t="shared" si="7"/>
-        <v>-0.94458740832705013</v>
-      </c>
-      <c r="G26" s="1">
-        <f>SUM(B26:F26)</f>
-        <v>-0.94458740832705079</v>
-      </c>
-      <c r="H26" s="1">
-        <f t="shared" si="8"/>
-        <v>-0.94458740832705113</v>
-      </c>
-      <c r="I26" s="1">
-        <f t="shared" si="10"/>
-        <v>-0.9446</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B27" s="1">
-        <f>B$8*(((E15-A$9)*(E15-A$10)*(E15-A$11)*(E15-A$12)*(E15-A$13))/((A$8-A$9)*(A$8-A$10)*(A$8-A$11)*(A$8-A$12)*(A$8-A$13)))</f>
-        <v>-0.91173391478696508</v>
-      </c>
-      <c r="C27" s="1">
-        <f>B$9*(((E15-A$8)*(E15-A$10)*(E15-A$11)*(E15-A$12)*(E15-A$13))/((A$9-A$8)*(A$9-A$10)*(A$9-A$11)*(A$9-A$12)*(A$9-A$13)))</f>
-        <v>0</v>
-      </c>
-      <c r="D27" s="1">
-        <f>B$10*(((E15-A$8)*(E15-A$9)*(E15-A$11)*(E15-A$12)*(E15-A$13))/((A$10-A$8)*(A$10-A$9)*(A$10-A$11)*(A$10-A$12)*(A$10-A$13)))</f>
-        <v>0</v>
-      </c>
-      <c r="E27" s="1">
-        <f>B$11*(((E15-A$8)*(E15-A$9)*(E15-A$10)*(E15-A$12)*(E15-A$13))/(($A$11-$A$8)*($A$11-$A$9)*($A$11-$A$10)*($A$11-$A$12)*($A$11-$A$13)))</f>
-        <v>0</v>
-      </c>
-      <c r="F27" s="1">
-        <f>$B$12*(((E15-$A$8)*(E15-$A$9)*(E15-$A$10)*(E15-$A$11)*(E15-$A$13))/(($A$12-$A$8)*($A$12-$A$9)*($A$12-$A$10)*($A$12-$A$11)*($A$12-$A$13)))</f>
-        <v>0</v>
-      </c>
-      <c r="G27" s="1">
-        <f t="shared" ref="G27" si="12">SUM(B27:F27)</f>
-        <v>-0.91173391478696508</v>
-      </c>
-      <c r="H27" s="1">
-        <f t="shared" si="8"/>
-        <v>-0.91173391478696508</v>
-      </c>
-      <c r="I27" s="1">
-        <f t="shared" si="10"/>
-        <v>-0.91169999999999995</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B29" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="G29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H29" s="1">
         <f>99375/240000</f>
         <v>0.4140625</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B30" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="G30" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H30" s="1">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="G25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H25" s="1">
         <f>-217250/240000</f>
         <v>-0.90520833333333328</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B31" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="G31" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H31" s="1">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="G26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H26" s="1">
         <f>217725/240000</f>
         <v>0.90718750000000004</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.45">
-      <c r="B32" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="G32" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H32" s="1">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="G27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H27" s="1">
         <f>-95890/240000</f>
         <v>-0.39954166666666668</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="B33" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="G33" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H33" s="1">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="G28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H28" s="1">
         <f>-218808/240000</f>
         <v>-0.91169999999999995</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B16:H16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2249,43 +2044,46 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF04314A-A607-4645-9456-8D51BB1A7663}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3984375" customWidth="1"/>
-    <col min="5" max="5" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="82.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2299,13 +2097,13 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="6"/>
       <c r="D6" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -2313,7 +2111,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -2327,19 +2125,19 @@
         <v>3</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -2371,7 +2169,7 @@
         <v>-1.0750080124661276E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f>A8+0.1</f>
         <v>4.0999999999999996</v>
@@ -2402,7 +2200,7 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" ref="A10:A12" si="3">A9+0.1</f>
         <v>4.1999999999999993</v>
@@ -2430,7 +2228,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="3"/>
         <v>4.2999999999999989</v>
@@ -2455,7 +2253,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f t="shared" si="3"/>
         <v>4.3999999999999986</v>
@@ -2477,21 +2275,45 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="I14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D15" s="1">
         <f>D8</f>
         <v>4</v>
@@ -2508,33 +2330,158 @@
         <f>(E15-D15)/F15</f>
         <v>3.9000000000000106</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="I15" s="1">
+        <f>D8</f>
+        <v>4</v>
+      </c>
+      <c r="J15" s="1">
+        <f>D4</f>
+        <v>4</v>
+      </c>
+      <c r="K15" s="1">
+        <f>D9-D8</f>
+        <v>9.9999999999999645E-2</v>
+      </c>
+      <c r="L15" s="1">
+        <f>(J15-I15)/K15</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="1">
+        <f>D8</f>
+        <v>4</v>
+      </c>
+      <c r="O15" s="1">
+        <f>E4</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="P15" s="1">
+        <f>D9-D8</f>
+        <v>9.9999999999999645E-2</v>
+      </c>
+      <c r="Q15" s="1">
+        <f>(O15-N15)/P15</f>
+        <v>4.0000000000000178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D17" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.45">
+      <c r="I17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" s="4"/>
+      <c r="N17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="O17" s="4"/>
+    </row>
+    <row r="18" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E18" s="1">
         <f>E8+F8*G15+G8*((G15*(G15-1))/2)+H8*((G15*(G15-1)*(G15-2))/6)+I8*((G15*(G15-1)*(G15-2)*(G15-3))/24)</f>
         <v>0.39499247355495709</v>
       </c>
+      <c r="I18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J18" s="1">
+        <f>(1/K15)*(F8+((2*L15-1)/2)*G8+((3*(L15^2)-6*L15+2)/6)*H8+((2*(L15^3)-9*(L15^2)+11*L15-3)/12)*I8)</f>
+        <v>1.3683942251486589</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O18" s="1">
+        <f>(1/(P15^2))*(G8+(Q15-1)*H8+((6*Q15^2-18*Q15+11)/12)*I8)</f>
+        <v>-0.35656028238193554</v>
+      </c>
+    </row>
+    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D21" s="1">
+        <f>C4</f>
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="E21" s="1">
+        <f>COS(D21+EXP(COS(D21)))</f>
+        <v>0.39499568104844979</v>
+      </c>
+      <c r="I21" s="1">
+        <f>D4</f>
+        <v>4</v>
+      </c>
+      <c r="J21" s="1">
+        <f>-SIN(I21+EXP(COS(I21)))*(1-SIN(I21)*EXP(COS(I21)))</f>
+        <v>1.3679753430261141</v>
+      </c>
+      <c r="N21" s="1">
+        <f>E4</f>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="O21" s="1">
+        <f>-COS(N21+EXP(COS(N21)))*((1-SIN(N21)*EXP(COS(N21)))^2)-SIN(N21+EXP(COS(N21)))*EXP(COS(N21))*((SIN(N21)^2)-COS(N21))</f>
+        <v>-0.37278652494317288</v>
+      </c>
+    </row>
+    <row r="23" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="1">
+        <f>ROUND(ABS(E18-E21), 4)</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J23" s="1">
+        <f>ROUND(ABS(J18-J21), 4)</f>
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O23" s="1">
+        <f>ROUND(ABS(O18-O21), 4)</f>
+        <v>1.6199999999999999E-2</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="D6:I6"/>
     <mergeCell ref="D17:E17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="N17:O17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>